<commit_message>
updating tables in supplementary
</commit_message>
<xml_diff>
--- a/ms/nature communications ms/Supplementary/Supplementary_model tables_S7-S13.xlsx
+++ b/ms/nature communications ms/Supplementary/Supplementary_model tables_S7-S13.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenharrison/Documents/GitHub/sex_meta/ms/nature communications ms/Supplementary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C82E975-6616-A544-8444-D21356D76769}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE7A78F-07C2-2542-A4B8-5528150140EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="38300" windowHeight="19760" activeTab="6" xr2:uid="{CEA959A6-D841-5347-BF8F-13749A5754E5}"/>
+    <workbookView xWindow="220" yWindow="500" windowWidth="38300" windowHeight="19760" xr2:uid="{CEA959A6-D841-5347-BF8F-13749A5754E5}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="7" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1865" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1865" uniqueCount="302">
   <si>
     <t>Birds</t>
   </si>
@@ -136,9 +136,6 @@
     <t>95% CI</t>
   </si>
   <si>
-    <t>p=0.76</t>
-  </si>
-  <si>
     <t>p=0.96</t>
   </si>
   <si>
@@ -238,15 +235,6 @@
     <t>-0.21, 0.72</t>
   </si>
   <si>
-    <t>p=0.86</t>
-  </si>
-  <si>
-    <t>-0.03, 0.51</t>
-  </si>
-  <si>
-    <t>-0.34, 0.28</t>
-  </si>
-  <si>
     <t>p=0.88</t>
   </si>
   <si>
@@ -262,15 +250,6 @@
     <t>-0.49, 0.33</t>
   </si>
   <si>
-    <t>p=0.81</t>
-  </si>
-  <si>
-    <t>-0.09, 0.06</t>
-  </si>
-  <si>
-    <t>-0.21, 0.16</t>
-  </si>
-  <si>
     <t>p=0.16</t>
   </si>
   <si>
@@ -298,12 +277,6 @@
     <t>-0.11, 0.22</t>
   </si>
   <si>
-    <t>-0.24, 0.54</t>
-  </si>
-  <si>
-    <t>-0.37, 0.73</t>
-  </si>
-  <si>
     <t>-0.34, 0.24</t>
   </si>
   <si>
@@ -316,15 +289,6 @@
     <t>-0.02, 0.19</t>
   </si>
   <si>
-    <t>p=0.59</t>
-  </si>
-  <si>
-    <t>-0.11, 0.12</t>
-  </si>
-  <si>
-    <t>-0.20, 0.13</t>
-  </si>
-  <si>
     <t>-0.25, 0.07</t>
   </si>
   <si>
@@ -343,12 +307,6 @@
     <t>-0.23, 0.34</t>
   </si>
   <si>
-    <t>-0.19, 0.81</t>
-  </si>
-  <si>
-    <t>-0.49, 0.36</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
@@ -364,15 +322,6 @@
     <t>-0.11, 0.24</t>
   </si>
   <si>
-    <t>p=0.64</t>
-  </si>
-  <si>
-    <t>-0.34, 0.18</t>
-  </si>
-  <si>
-    <t>-0.19, 0.31</t>
-  </si>
-  <si>
     <t>p=0.44</t>
   </si>
   <si>
@@ -535,9 +484,6 @@
     <t>S11 - Contrast models for each of the five taxonomic groups with study type (observation vs experimental) as moderator. Note there were no observational studies for invertebrates so they have not been included.</t>
   </si>
   <si>
-    <t xml:space="preserve">S12 - Assessing publication bias. Full models (personality trait MLMR models) with precision as moderator term. </t>
-  </si>
-  <si>
     <t>QE - scores in MLMR model tables are tests of residual heterogeneity (heterogeneity not explained by moderators in model)</t>
   </si>
   <si>
@@ -935,6 +881,63 @@
   </si>
   <si>
     <t>-0.17, 0.68</t>
+  </si>
+  <si>
+    <t>p=0.51</t>
+  </si>
+  <si>
+    <t>-0.02, 0.63</t>
+  </si>
+  <si>
+    <t>-0.48, 0.24</t>
+  </si>
+  <si>
+    <t>p=0.78</t>
+  </si>
+  <si>
+    <t>-0.11, 0.10</t>
+  </si>
+  <si>
+    <t>-0.19, 0.25</t>
+  </si>
+  <si>
+    <t>p=0.33</t>
+  </si>
+  <si>
+    <t>-0.30, 0.59</t>
+  </si>
+  <si>
+    <t>-0.33, 0.97</t>
+  </si>
+  <si>
+    <t>p=0.38</t>
+  </si>
+  <si>
+    <t>-0.10, 0.16</t>
+  </si>
+  <si>
+    <t>-0.26, 0.10</t>
+  </si>
+  <si>
+    <t>p=0.77</t>
+  </si>
+  <si>
+    <t>-0.19, 0.92</t>
+  </si>
+  <si>
+    <t>-0.52, 0.39</t>
+  </si>
+  <si>
+    <t>p=0.66</t>
+  </si>
+  <si>
+    <t>-0.34, 0.22</t>
+  </si>
+  <si>
+    <t>-0.21, 0.33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S12 - Assessing publication bias. Full models (personality trait MLMR models) with precision as additional moderator term. </t>
   </si>
 </sst>
 </file>
@@ -1404,90 +1407,90 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{997D318C-6FE4-1349-B40F-3ACEE7BB8369}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>301</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1499,7 +1502,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9948B2D6-0D24-AC4F-B3C7-22D23935FFEB}">
   <dimension ref="A1:AN60"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1513,23 +1518,23 @@
   <sheetData>
     <row r="1" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:40" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -1656,7 +1661,7 @@
         <v>0.17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="D8" s="5"/>
       <c r="I8" s="5" t="s">
@@ -1666,7 +1671,7 @@
         <v>0.68</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q8" s="5" t="s">
         <v>8</v>
@@ -1675,7 +1680,7 @@
         <v>0</v>
       </c>
       <c r="S8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>8</v>
@@ -1684,7 +1689,7 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="AG8" s="5" t="s">
         <v>8</v>
@@ -1693,7 +1698,7 @@
         <v>0.54</v>
       </c>
       <c r="AI8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
@@ -2174,13 +2179,13 @@
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16">
         <v>-0.15</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="D16">
         <v>-1.23</v>
@@ -2198,13 +2203,13 @@
         <v>43</v>
       </c>
       <c r="I16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J16" s="28">
         <v>0.08</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L16" s="28">
         <v>0.42</v>
@@ -2222,13 +2227,13 @@
         <v>8</v>
       </c>
       <c r="Q16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R16">
         <v>0.23</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T16">
         <v>0.68</v>
@@ -2237,7 +2242,7 @@
         <v>0.5</v>
       </c>
       <c r="V16">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="W16">
         <v>3</v>
@@ -2246,13 +2251,13 @@
         <v>3</v>
       </c>
       <c r="Y16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Z16" s="5">
         <v>-0.08</v>
       </c>
       <c r="AA16" s="11" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="AB16" s="5">
         <v>-0.28000000000000003</v>
@@ -2270,13 +2275,13 @@
         <v>9</v>
       </c>
       <c r="AG16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH16" s="28">
         <v>0.23</v>
       </c>
       <c r="AI16" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AJ16" s="28">
         <v>0.65</v>
@@ -2296,13 +2301,13 @@
     </row>
     <row r="17" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="13">
         <v>0.08</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="D17" s="13">
         <v>0.41</v>
@@ -2320,13 +2325,13 @@
         <v>9</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J17" s="13">
         <v>-0.11</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L17" s="13">
         <v>-0.83</v>
@@ -2344,13 +2349,13 @@
         <v>34</v>
       </c>
       <c r="Q17" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R17" s="15">
         <v>0.02</v>
       </c>
       <c r="S17" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="T17" s="15">
         <v>0.05</v>
@@ -2359,22 +2364,22 @@
         <v>0.96</v>
       </c>
       <c r="V17" s="15">
-        <v>427</v>
+        <v>368</v>
       </c>
       <c r="W17" s="15">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="X17" s="15">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="Y17" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Z17" s="13">
         <v>0.16</v>
       </c>
       <c r="AA17" s="14" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="AB17" s="13">
         <v>1.07</v>
@@ -2392,13 +2397,13 @@
         <v>52</v>
       </c>
       <c r="AG17" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH17" s="15">
         <v>-0.26</v>
       </c>
       <c r="AI17" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AJ17" s="15">
         <v>-0.74</v>
@@ -2477,7 +2482,7 @@
         <v>52.82</v>
       </c>
       <c r="AI19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.2">
@@ -2488,7 +2493,7 @@
         <v>0.04</v>
       </c>
       <c r="C20" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>8</v>
@@ -2497,7 +2502,7 @@
         <v>0.02</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q20" s="5" t="s">
         <v>8</v>
@@ -2506,7 +2511,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y20" s="5" t="s">
         <v>8</v>
@@ -2515,7 +2520,7 @@
         <v>0.32</v>
       </c>
       <c r="AA20" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="AG20" s="5" t="s">
         <v>8</v>
@@ -2524,7 +2529,7 @@
         <v>0.02</v>
       </c>
       <c r="AI20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.2">
@@ -3004,13 +3009,13 @@
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="7">
         <v>-0.16</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="D28" s="7">
         <v>-0.57999999999999996</v>
@@ -3028,13 +3033,13 @@
         <v>43</v>
       </c>
       <c r="I28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J28" s="26">
         <v>-0.04</v>
       </c>
       <c r="K28" s="27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L28" s="26">
         <v>-0.64</v>
@@ -3052,13 +3057,13 @@
         <v>8</v>
       </c>
       <c r="Q28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R28">
         <v>0.04</v>
       </c>
       <c r="S28" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T28">
         <v>0.26</v>
@@ -3067,7 +3072,7 @@
         <v>0.8</v>
       </c>
       <c r="V28">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="W28">
         <v>3</v>
@@ -3076,13 +3081,13 @@
         <v>3</v>
       </c>
       <c r="Y28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Z28" s="7">
         <v>0.03</v>
       </c>
       <c r="AA28" s="17" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="AB28" s="7">
         <v>0.2</v>
@@ -3100,13 +3105,13 @@
         <v>9</v>
       </c>
       <c r="AG28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH28" s="7">
         <v>-0.03</v>
       </c>
       <c r="AI28" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AJ28" s="7">
         <v>-0.14000000000000001</v>
@@ -3126,13 +3131,13 @@
     </row>
     <row r="29" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" s="15">
         <v>0.05</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="D29" s="15">
         <v>0.2</v>
@@ -3150,13 +3155,13 @@
         <v>9</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J29" s="13">
         <v>0.01</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L29" s="13">
         <v>0.12</v>
@@ -3174,13 +3179,13 @@
         <v>34</v>
       </c>
       <c r="Q29" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R29" s="15">
         <v>-0.06</v>
       </c>
       <c r="S29" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="T29" s="15">
         <v>-0.37</v>
@@ -3189,22 +3194,22 @@
         <v>0.71</v>
       </c>
       <c r="V29" s="15">
-        <v>427</v>
+        <v>368</v>
       </c>
       <c r="W29" s="15">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="X29" s="15">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="Y29" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Z29" s="15">
         <v>0.05</v>
       </c>
       <c r="AA29" s="16" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="AB29" s="15">
         <v>0.56999999999999995</v>
@@ -3222,13 +3227,13 @@
         <v>52</v>
       </c>
       <c r="AG29" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH29" s="15">
         <v>0.03</v>
       </c>
       <c r="AI29" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AJ29" s="15">
         <v>0.14000000000000001</v>
@@ -3358,8 +3363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345FC792-B22C-5445-AAC6-18CE35CE0157}">
   <dimension ref="A1:AN68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AD25" sqref="AD25"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3373,23 +3378,23 @@
   <sheetData>
     <row r="1" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:40" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -3484,7 +3489,7 @@
         <v>6</v>
       </c>
       <c r="R7">
-        <v>2891.35</v>
+        <v>2677.09</v>
       </c>
       <c r="S7" t="s">
         <v>7</v>
@@ -3516,7 +3521,7 @@
         <v>0.01</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>8</v>
@@ -3531,10 +3536,10 @@
         <v>8</v>
       </c>
       <c r="R8">
-        <v>0.03</v>
+        <v>0.42</v>
       </c>
       <c r="S8" t="s">
-        <v>68</v>
+        <v>283</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>8</v>
@@ -3543,7 +3548,7 @@
         <v>0.93</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="AG8" s="5" t="s">
         <v>8</v>
@@ -3552,7 +3557,7 @@
         <v>0.02</v>
       </c>
       <c r="AI8" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
@@ -3709,13 +3714,13 @@
         <v>13</v>
       </c>
       <c r="R11">
-        <v>0.75</v>
+        <v>0.9</v>
       </c>
       <c r="S11">
-        <v>0.87</v>
+        <v>0.95</v>
       </c>
       <c r="T11">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="U11" s="4"/>
       <c r="Y11" t="s">
@@ -3778,7 +3783,7 @@
         <v>0</v>
       </c>
       <c r="T12">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Y12" t="s">
         <v>14</v>
@@ -3834,13 +3839,13 @@
         <v>15</v>
       </c>
       <c r="R13">
-        <v>0.27</v>
+        <v>0.32</v>
       </c>
       <c r="S13">
-        <v>0.52</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="T13">
-        <v>483</v>
+        <v>422</v>
       </c>
       <c r="Y13" t="s">
         <v>15</v>
@@ -4033,13 +4038,13 @@
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16">
         <v>-0.13</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D16">
         <v>-1.1399999999999999</v>
@@ -4057,13 +4062,13 @@
         <v>43</v>
       </c>
       <c r="I16" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J16" s="28">
         <v>-0.05</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L16" s="28">
         <v>-0.3</v>
@@ -4080,32 +4085,32 @@
       <c r="P16" s="28">
         <v>43</v>
       </c>
-      <c r="Q16" s="18" t="s">
+      <c r="Q16" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="R16" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="S16" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="T16" s="5">
+        <v>1.86</v>
+      </c>
+      <c r="U16" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="V16" s="5">
+        <v>381</v>
+      </c>
+      <c r="W16" s="5">
+        <v>35</v>
+      </c>
+      <c r="X16" s="5">
         <v>36</v>
       </c>
-      <c r="R16" s="4">
-        <v>0.24</v>
-      </c>
-      <c r="S16" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="T16" s="4">
-        <v>1.74</v>
-      </c>
-      <c r="U16" s="4">
-        <v>0.08</v>
-      </c>
-      <c r="V16" s="4">
-        <v>439</v>
-      </c>
-      <c r="W16" s="4">
-        <v>39</v>
-      </c>
-      <c r="X16" s="4">
-        <v>42</v>
-      </c>
       <c r="Y16" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Z16" s="5">
         <v>0.1</v>
@@ -4129,13 +4134,13 @@
         <v>48</v>
       </c>
       <c r="AG16" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH16" s="28">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AI16" s="10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="AJ16" s="28">
         <v>0.87</v>
@@ -4155,13 +4160,13 @@
     </row>
     <row r="17" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="13">
         <v>-0.01</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="D17" s="13">
         <v>-0.08</v>
@@ -4179,13 +4184,13 @@
         <v>13</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J17" s="13">
         <v>0.26</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L17" s="13">
         <v>1.08</v>
@@ -4203,37 +4208,37 @@
         <v>3</v>
       </c>
       <c r="Q17" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R17" s="15">
-        <v>-0.03</v>
+        <v>-0.12</v>
       </c>
       <c r="S17" s="16" t="s">
-        <v>70</v>
+        <v>285</v>
       </c>
       <c r="T17" s="15">
-        <v>-0.18</v>
+        <v>-0.65</v>
       </c>
       <c r="U17" s="15">
-        <v>0.86</v>
+        <v>0.51</v>
       </c>
       <c r="V17" s="15">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="W17" s="15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X17" s="15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Y17" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Z17" s="13">
         <v>-0.09</v>
       </c>
       <c r="AA17" s="14" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="AB17" s="13">
         <v>-0.96</v>
@@ -4251,13 +4256,13 @@
         <v>19</v>
       </c>
       <c r="AG17" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AH17" s="15">
         <v>-0.05</v>
       </c>
       <c r="AI17" s="16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="AJ17" s="15">
         <v>-0.16</v>
@@ -4315,7 +4320,7 @@
         <v>6</v>
       </c>
       <c r="R19">
-        <v>1537.49</v>
+        <v>1459.48</v>
       </c>
       <c r="S19" t="s">
         <v>7</v>
@@ -4336,7 +4341,7 @@
         <v>77.59</v>
       </c>
       <c r="AI19" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.2">
@@ -4347,7 +4352,7 @@
         <v>0.06</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>8</v>
@@ -4362,10 +4367,10 @@
         <v>8</v>
       </c>
       <c r="R20">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>76</v>
+        <v>286</v>
       </c>
       <c r="Y20" s="5" t="s">
         <v>8</v>
@@ -4374,7 +4379,7 @@
         <v>2.23</v>
       </c>
       <c r="AA20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AG20" s="5" t="s">
         <v>8</v>
@@ -4383,7 +4388,7 @@
         <v>0.15</v>
       </c>
       <c r="AI20" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.2">
@@ -4542,10 +4547,10 @@
         <v>0.04</v>
       </c>
       <c r="S23">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="T23">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="Y23" t="s">
         <v>13</v>
@@ -4604,10 +4609,10 @@
         <v>0</v>
       </c>
       <c r="S24">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="T24">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Y24" t="s">
         <v>14</v>
@@ -4664,13 +4669,13 @@
         <v>15</v>
       </c>
       <c r="R25">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="S25">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
       <c r="T25">
-        <v>483</v>
+        <v>422</v>
       </c>
       <c r="Y25" t="s">
         <v>15</v>
@@ -4863,13 +4868,13 @@
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="7">
         <v>-0.14000000000000001</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="D28" s="7">
         <v>-0.53</v>
@@ -4887,13 +4892,13 @@
         <v>43</v>
       </c>
       <c r="I28" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J28" s="26">
         <v>-0.04</v>
       </c>
       <c r="K28" s="27" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="L28" s="26">
         <v>-1.38</v>
@@ -4911,37 +4916,37 @@
         <v>43</v>
       </c>
       <c r="Q28" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="T28">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="U28">
+        <v>0.94</v>
+      </c>
+      <c r="V28" s="5">
+        <v>381</v>
+      </c>
+      <c r="W28" s="5">
+        <v>35</v>
+      </c>
+      <c r="X28" s="5">
         <v>36</v>
       </c>
-      <c r="R28">
-        <v>-0.02</v>
-      </c>
-      <c r="S28" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="T28">
-        <v>-0.39</v>
-      </c>
-      <c r="U28">
-        <v>0.7</v>
-      </c>
-      <c r="V28" s="5">
-        <v>439</v>
-      </c>
-      <c r="W28" s="5">
-        <v>39</v>
-      </c>
-      <c r="X28" s="5">
-        <v>42</v>
-      </c>
       <c r="Y28" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Z28" s="7">
         <v>0.09</v>
       </c>
       <c r="AA28" s="17" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="AB28" s="7">
         <v>0.75</v>
@@ -4959,13 +4964,13 @@
         <v>48</v>
       </c>
       <c r="AG28" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH28" s="7">
         <v>0.06</v>
       </c>
       <c r="AI28" s="17" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="AJ28" s="7">
         <v>1.1399999999999999</v>
@@ -4985,13 +4990,13 @@
     </row>
     <row r="29" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="13">
         <v>-0.03</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="D29" s="13">
         <v>-0.25</v>
@@ -5009,13 +5014,13 @@
         <v>13</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J29" s="13">
         <v>-0.08</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L29" s="13">
         <v>-0.37</v>
@@ -5033,37 +5038,37 @@
         <v>3</v>
       </c>
       <c r="Q29" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R29" s="15">
-        <v>-0.02</v>
+        <v>0.03</v>
       </c>
       <c r="S29" s="16" t="s">
-        <v>78</v>
+        <v>288</v>
       </c>
       <c r="T29" s="15">
-        <v>-0.24</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="U29" s="15">
-        <v>0.81</v>
+        <v>0.78</v>
       </c>
       <c r="V29" s="13">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="W29" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X29" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Y29" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Z29" s="15">
         <v>-0.1</v>
       </c>
       <c r="AA29" s="16" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="AB29" s="15">
         <v>-1.49</v>
@@ -5081,13 +5086,13 @@
         <v>19</v>
       </c>
       <c r="AG29" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AH29" s="15">
         <v>-0.08</v>
       </c>
       <c r="AI29" s="16" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="AJ29" s="15">
         <v>-0.39</v>
@@ -5565,8 +5570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A46B4CE2-FDF2-D946-A9CE-F47AE9C974AB}">
   <dimension ref="A1:AN35"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5580,23 +5585,23 @@
   <sheetData>
     <row r="1" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:40" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -5691,7 +5696,7 @@
         <v>6</v>
       </c>
       <c r="R7">
-        <v>2873.93</v>
+        <v>2671.64</v>
       </c>
       <c r="S7" t="s">
         <v>7</v>
@@ -5723,7 +5728,7 @@
         <v>0.12</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>8</v>
@@ -5732,16 +5737,16 @@
         <v>0.36</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="R8" s="5">
-        <v>0.41</v>
+        <v>0.96</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>44</v>
+        <v>289</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>8</v>
@@ -5750,7 +5755,7 @@
         <v>1.99</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="AG8" s="5" t="s">
         <v>8</v>
@@ -5759,7 +5764,7 @@
         <v>0.1</v>
       </c>
       <c r="AI8" s="5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
@@ -5916,13 +5921,13 @@
         <v>13</v>
       </c>
       <c r="R11">
-        <v>0.77</v>
+        <v>0.91</v>
       </c>
       <c r="S11">
-        <v>0.88</v>
+        <v>0.95</v>
       </c>
       <c r="T11" s="5">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="U11" s="4"/>
       <c r="Y11" t="s">
@@ -5985,7 +5990,7 @@
         <v>0</v>
       </c>
       <c r="T12">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Y12" t="s">
         <v>14</v>
@@ -6041,13 +6046,13 @@
         <v>15</v>
       </c>
       <c r="R13">
-        <v>0.27</v>
+        <v>0.31</v>
       </c>
       <c r="S13">
-        <v>0.52</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="T13">
-        <v>483</v>
+        <v>422</v>
       </c>
       <c r="Y13" t="s">
         <v>15</v>
@@ -6240,13 +6245,13 @@
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16">
         <v>-0.16</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="D16">
         <v>-1.1499999999999999</v>
@@ -6264,13 +6269,13 @@
         <v>34</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J16">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="L16">
         <v>-0.4</v>
@@ -6288,37 +6293,37 @@
         <v>17</v>
       </c>
       <c r="Q16" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R16">
-        <v>0.15</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>88</v>
+        <v>290</v>
       </c>
       <c r="T16">
-        <v>0.76</v>
+        <v>0.63</v>
       </c>
       <c r="U16">
-        <v>0.45</v>
+        <v>0.53</v>
       </c>
       <c r="V16">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="W16">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="X16">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="Y16" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Z16" s="5">
         <v>0.16</v>
       </c>
       <c r="AA16" s="11" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="AB16" s="5">
         <v>0.96</v>
@@ -6336,13 +6341,13 @@
         <v>26</v>
       </c>
       <c r="AG16" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH16">
         <v>0.08</v>
       </c>
       <c r="AI16" s="10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="AJ16">
         <v>0.92</v>
@@ -6362,13 +6367,13 @@
     </row>
     <row r="17" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B17" s="13">
         <v>0.09</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="D17" s="13">
         <v>0.35</v>
@@ -6386,13 +6391,13 @@
         <v>16</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="J17" s="13">
         <v>0.05</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="L17" s="13">
         <v>0.6</v>
@@ -6410,37 +6415,37 @@
         <v>28</v>
       </c>
       <c r="Q17" s="13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="R17" s="15">
-        <v>0.18</v>
+        <v>0.32</v>
       </c>
       <c r="S17" s="16" t="s">
-        <v>89</v>
+        <v>291</v>
       </c>
       <c r="T17" s="15">
-        <v>0.64</v>
+        <v>0.98</v>
       </c>
       <c r="U17" s="15">
-        <v>0.52</v>
+        <v>0.33</v>
       </c>
       <c r="V17" s="15">
-        <v>294</v>
+        <v>245</v>
       </c>
       <c r="W17" s="15">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="X17" s="15">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="Y17" s="13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="Z17" s="13">
         <v>-0.15</v>
       </c>
       <c r="AA17" s="14" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="AB17" s="13">
         <v>-1.41</v>
@@ -6458,13 +6463,13 @@
         <v>36</v>
       </c>
       <c r="AG17" s="13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="AH17" s="15">
         <v>-0.05</v>
       </c>
       <c r="AI17" s="16" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="AJ17" s="15">
         <v>-0.32</v>
@@ -6522,7 +6527,7 @@
         <v>6</v>
       </c>
       <c r="R19">
-        <v>1538.04</v>
+        <v>1459.07</v>
       </c>
       <c r="S19" t="s">
         <v>7</v>
@@ -6543,7 +6548,7 @@
         <v>77.27</v>
       </c>
       <c r="AI19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.2">
@@ -6554,7 +6559,7 @@
         <v>0.52</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>8</v>
@@ -6563,16 +6568,16 @@
         <v>2.39</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="Q20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="R20" s="5">
-        <v>0.28999999999999998</v>
+        <v>0.76</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>94</v>
+        <v>292</v>
       </c>
       <c r="Y20" s="5" t="s">
         <v>8</v>
@@ -6590,7 +6595,7 @@
         <v>0.42</v>
       </c>
       <c r="AI20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.2">
@@ -6746,13 +6751,13 @@
         <v>13</v>
       </c>
       <c r="R23">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="S23">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="T23" s="5">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="Y23" t="s">
         <v>13</v>
@@ -6811,10 +6816,10 @@
         <v>0</v>
       </c>
       <c r="S24">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="T24">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Y24" t="s">
         <v>14</v>
@@ -6871,13 +6876,13 @@
         <v>15</v>
       </c>
       <c r="R25">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="S25">
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
       <c r="T25">
-        <v>483</v>
+        <v>422</v>
       </c>
       <c r="Y25" t="s">
         <v>15</v>
@@ -7070,13 +7075,13 @@
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="7">
         <v>-0.1</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="D28" s="7">
         <v>-0.87</v>
@@ -7094,13 +7099,13 @@
         <v>34</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J28" s="18">
         <v>-0.09</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="L28" s="18">
         <v>-2.11</v>
@@ -7118,37 +7123,37 @@
         <v>17</v>
       </c>
       <c r="Q28" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R28" s="26">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="S28" s="27" t="s">
-        <v>95</v>
+        <v>293</v>
       </c>
       <c r="T28" s="26">
-        <v>0.1</v>
+        <v>0.45</v>
       </c>
       <c r="U28" s="26">
-        <v>0.92</v>
+        <v>0.66</v>
       </c>
       <c r="V28">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="W28">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="X28">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="Y28" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Z28" s="7">
         <v>0.11</v>
       </c>
       <c r="AA28" s="17" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="AB28" s="7">
         <v>0.7</v>
@@ -7166,13 +7171,13 @@
         <v>26</v>
       </c>
       <c r="AG28" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH28" s="7">
         <v>0.06</v>
       </c>
       <c r="AI28" s="17" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="AJ28" s="7">
         <v>1.18</v>
@@ -7192,13 +7197,13 @@
     </row>
     <row r="29" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B29" s="13">
         <v>0.14000000000000001</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="D29" s="13">
         <v>0.72</v>
@@ -7216,13 +7221,13 @@
         <v>16</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="J29" s="13">
         <v>0.08</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="L29" s="13">
         <v>1.55</v>
@@ -7240,37 +7245,37 @@
         <v>28</v>
       </c>
       <c r="Q29" s="13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="R29" s="13">
-        <v>-0.04</v>
+        <v>-0.08</v>
       </c>
       <c r="S29" s="14" t="s">
-        <v>96</v>
+        <v>294</v>
       </c>
       <c r="T29" s="13">
-        <v>-0.54</v>
+        <v>-0.87</v>
       </c>
       <c r="U29" s="13">
-        <v>0.59</v>
+        <v>0.38</v>
       </c>
       <c r="V29" s="15">
-        <v>294</v>
+        <v>245</v>
       </c>
       <c r="W29" s="15">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="X29" s="15">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="Y29" s="13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="Z29" s="15">
         <v>-0.09</v>
       </c>
       <c r="AA29" s="16" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="AB29" s="15">
         <v>-1.07</v>
@@ -7288,13 +7293,13 @@
         <v>36</v>
       </c>
       <c r="AG29" s="13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="AH29" s="15">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="AI29" s="16" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="AJ29" s="15">
         <v>-0.65</v>
@@ -7330,31 +7335,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FBA234-D4FE-CE44-A5C8-7BF7641E4438}">
   <dimension ref="A1:AN35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AO17" sqref="AO17"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:40" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -7449,7 +7454,7 @@
         <v>6</v>
       </c>
       <c r="R7">
-        <v>2891.27</v>
+        <v>2677.88</v>
       </c>
       <c r="S7" t="s">
         <v>7</v>
@@ -7481,7 +7486,7 @@
         <v>0.01</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>8</v>
@@ -7490,16 +7495,16 @@
         <v>0.15</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="Q8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="R8" s="5">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>34</v>
+        <v>295</v>
       </c>
       <c r="Y8" s="4" t="s">
         <v>8</v>
@@ -7511,7 +7516,7 @@
         <v>25</v>
       </c>
       <c r="AB8" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="AG8" s="5" t="s">
         <v>8</v>
@@ -7520,7 +7525,7 @@
         <v>2.9</v>
       </c>
       <c r="AI8" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
@@ -7677,13 +7682,13 @@
         <v>13</v>
       </c>
       <c r="R11">
-        <v>0.75</v>
+        <v>0.9</v>
       </c>
       <c r="S11">
-        <v>0.87</v>
+        <v>0.95</v>
       </c>
       <c r="T11" s="5">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="U11" s="4"/>
       <c r="Y11" t="s">
@@ -7746,7 +7751,7 @@
         <v>0</v>
       </c>
       <c r="T12">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Y12" t="s">
         <v>14</v>
@@ -7802,13 +7807,13 @@
         <v>15</v>
       </c>
       <c r="R13">
-        <v>0.27</v>
+        <v>0.32</v>
       </c>
       <c r="S13">
-        <v>0.52</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="T13">
-        <v>483</v>
+        <v>422</v>
       </c>
       <c r="Y13" t="s">
         <v>15</v>
@@ -8001,13 +8006,13 @@
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16">
         <v>-0.13</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="D16">
         <v>-0.92</v>
@@ -8025,13 +8030,13 @@
         <v>29</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J16">
         <v>-0.06</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="L16">
         <v>-0.35</v>
@@ -8049,19 +8054,19 @@
         <v>5</v>
       </c>
       <c r="Q16" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R16">
-        <v>0.31</v>
+        <v>0.36</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>103</v>
+        <v>296</v>
       </c>
       <c r="T16">
-        <v>1.2</v>
+        <v>1.29</v>
       </c>
       <c r="U16">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="V16">
         <v>14</v>
@@ -8073,13 +8078,13 @@
         <v>1</v>
       </c>
       <c r="Y16" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Z16" s="5">
         <v>0.24</v>
       </c>
       <c r="AA16" s="11" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="AB16" s="5">
         <v>1.38</v>
@@ -8097,13 +8102,13 @@
         <v>22</v>
       </c>
       <c r="AG16" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH16">
         <v>-0.28999999999999998</v>
       </c>
       <c r="AI16" s="10" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="AJ16">
         <v>-1.24</v>
@@ -8123,13 +8128,13 @@
     </row>
     <row r="17" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B17" s="13">
         <v>-0.01</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D17" s="13">
         <v>-0.08</v>
@@ -8147,13 +8152,13 @@
         <v>22</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="J17" s="13">
         <v>0.06</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L17" s="13">
         <v>0.39</v>
@@ -8171,37 +8176,37 @@
         <v>39</v>
       </c>
       <c r="Q17" s="13" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="R17" s="15">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="S17" s="16" t="s">
-        <v>104</v>
+        <v>297</v>
       </c>
       <c r="T17" s="15">
-        <v>-0.31</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="U17" s="15">
-        <v>0.76</v>
+        <v>0.77</v>
       </c>
       <c r="V17" s="15">
-        <v>469</v>
+        <v>408</v>
       </c>
       <c r="W17" s="15">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="X17" s="15">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="Y17" s="29" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="Z17" s="29">
         <v>-0.3</v>
       </c>
       <c r="AA17" s="30" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="AB17" s="29">
         <v>-2.2599999999999998</v>
@@ -8218,28 +8223,28 @@
       <c r="AF17" s="29">
         <v>40</v>
       </c>
-      <c r="AG17" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="AH17" s="29">
+      <c r="AG17" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH17" s="13">
         <v>0.42</v>
       </c>
-      <c r="AI17" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="AJ17" s="29">
+      <c r="AI17" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ17" s="13">
         <v>1.7</v>
       </c>
-      <c r="AK17" s="29">
+      <c r="AK17" s="13">
         <v>0.09</v>
       </c>
-      <c r="AL17" s="29">
+      <c r="AL17" s="13">
         <v>90</v>
       </c>
-      <c r="AM17" s="29">
+      <c r="AM17" s="13">
         <v>8</v>
       </c>
-      <c r="AN17" s="29">
+      <c r="AN17" s="13">
         <v>9</v>
       </c>
     </row>
@@ -8283,7 +8288,7 @@
         <v>6</v>
       </c>
       <c r="R19">
-        <v>1539.06</v>
+        <v>1458.05</v>
       </c>
       <c r="S19" t="s">
         <v>7</v>
@@ -8304,7 +8309,7 @@
         <v>77.55</v>
       </c>
       <c r="AI19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.2">
@@ -8315,7 +8320,7 @@
         <v>0.81</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>8</v>
@@ -8324,16 +8329,16 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="R20" s="5">
-        <v>0.23</v>
+        <v>0.19</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>110</v>
+        <v>298</v>
       </c>
       <c r="Y20" s="5" t="s">
         <v>8</v>
@@ -8342,7 +8347,7 @@
         <v>0.47</v>
       </c>
       <c r="AA20" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="AG20" s="5" t="s">
         <v>8</v>
@@ -8351,7 +8356,7 @@
         <v>0.23</v>
       </c>
       <c r="AI20" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.2">
@@ -8510,10 +8515,10 @@
         <v>0.04</v>
       </c>
       <c r="S23">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="T23" s="5">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="Y23" t="s">
         <v>13</v>
@@ -8572,10 +8577,10 @@
         <v>0</v>
       </c>
       <c r="S24">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T24">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Y24" t="s">
         <v>14</v>
@@ -8632,13 +8637,13 @@
         <v>15</v>
       </c>
       <c r="R25">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="S25">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
       <c r="T25">
-        <v>483</v>
+        <v>422</v>
       </c>
       <c r="Y25" t="s">
         <v>15</v>
@@ -8831,13 +8836,13 @@
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="7">
         <v>-0.12</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="D28" s="7">
         <v>-1.01</v>
@@ -8855,13 +8860,13 @@
         <v>29</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J28" s="26">
         <v>-0.1</v>
       </c>
       <c r="K28" s="27" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="L28" s="26">
         <v>-1.18</v>
@@ -8879,19 +8884,19 @@
         <v>5</v>
       </c>
       <c r="Q28" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R28" s="26">
-        <v>-0.08</v>
+        <v>-0.06</v>
       </c>
       <c r="S28" s="27" t="s">
-        <v>111</v>
+        <v>299</v>
       </c>
       <c r="T28" s="26">
-        <v>-0.57999999999999996</v>
+        <v>-0.42</v>
       </c>
       <c r="U28" s="26">
-        <v>0.56000000000000005</v>
+        <v>0.67</v>
       </c>
       <c r="V28">
         <v>14</v>
@@ -8903,13 +8908,13 @@
         <v>1</v>
       </c>
       <c r="Y28" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Z28" s="7">
         <v>0.1</v>
       </c>
       <c r="AA28" s="17" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="AB28" s="7">
         <v>0.68</v>
@@ -8927,13 +8932,13 @@
         <v>22</v>
       </c>
       <c r="AG28" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH28" s="7">
         <v>-0.01</v>
       </c>
       <c r="AI28" s="17" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="AJ28" s="7">
         <v>-7.0000000000000007E-2</v>
@@ -8953,13 +8958,13 @@
     </row>
     <row r="29" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B29" s="13">
         <v>0.15</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="D29" s="13">
         <v>0.9</v>
@@ -8977,13 +8982,13 @@
         <v>22</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="J29" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="L29" s="13">
         <v>0.75</v>
@@ -9001,37 +9006,37 @@
         <v>39</v>
       </c>
       <c r="Q29" s="13" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="R29" s="13">
         <v>0.06</v>
       </c>
       <c r="S29" s="14" t="s">
-        <v>112</v>
+        <v>300</v>
       </c>
       <c r="T29" s="13">
-        <v>0.47</v>
+        <v>0.44</v>
       </c>
       <c r="U29" s="13">
-        <v>0.64</v>
+        <v>0.66</v>
       </c>
       <c r="V29" s="15">
-        <v>469</v>
+        <v>408</v>
       </c>
       <c r="W29" s="15">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="X29" s="15">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="Y29" s="13" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="Z29" s="15">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="AA29" s="16" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="AB29" s="15">
         <v>-0.69</v>
@@ -9049,13 +9054,13 @@
         <v>40</v>
       </c>
       <c r="AG29" s="13" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="AH29" s="15">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AI29" s="16" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="AJ29" s="15">
         <v>0.48</v>
@@ -9092,7 +9097,7 @@
   <dimension ref="A1:AN35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9106,23 +9111,23 @@
   <sheetData>
     <row r="1" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:40" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -9246,7 +9251,7 @@
         <v>1.31</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>8</v>
@@ -9255,7 +9260,7 @@
         <v>1.38</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="Q8" s="5" t="s">
         <v>8</v>
@@ -9270,10 +9275,10 @@
         <v>7.91</v>
       </c>
       <c r="AA8" s="4" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="AB8" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="AG8" s="5" t="s">
         <v>8</v>
@@ -9282,7 +9287,7 @@
         <v>2.9</v>
       </c>
       <c r="AI8" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
@@ -9763,13 +9768,13 @@
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16">
         <v>-0.04</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="D16">
         <v>-0.26</v>
@@ -9787,13 +9792,13 @@
         <v>32</v>
       </c>
       <c r="I16" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J16" s="28">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="L16" s="28">
         <v>-0.41</v>
@@ -9811,7 +9816,7 @@
         <v>19</v>
       </c>
       <c r="Q16" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R16" t="s">
         <v>26</v>
@@ -9835,13 +9840,13 @@
         <v>26</v>
       </c>
       <c r="Y16" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Z16" s="5">
         <v>0</v>
       </c>
       <c r="AA16" s="11" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="AB16" s="5">
         <v>0.04</v>
@@ -9859,13 +9864,13 @@
         <v>47</v>
       </c>
       <c r="AG16" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH16" s="28">
         <v>0.13</v>
       </c>
       <c r="AI16" s="10" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="AJ16" s="28">
         <v>1.1399999999999999</v>
@@ -9885,13 +9890,13 @@
     </row>
     <row r="17" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B17" s="13">
         <v>-0.28000000000000003</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="D17" s="13">
         <v>-1.1499999999999999</v>
@@ -9909,13 +9914,13 @@
         <v>18</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="J17" s="13">
         <v>0.19</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="L17" s="13">
         <v>1.17</v>
@@ -9933,7 +9938,7 @@
         <v>3</v>
       </c>
       <c r="Q17" s="13" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="R17" s="15" t="s">
         <v>26</v>
@@ -9957,13 +9962,13 @@
         <v>26</v>
       </c>
       <c r="Y17" s="29" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="Z17" s="29">
         <v>0.38</v>
       </c>
       <c r="AA17" s="30" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="AB17" s="29">
         <v>2.81</v>
@@ -9980,28 +9985,28 @@
       <c r="AF17" s="29">
         <v>14</v>
       </c>
-      <c r="AG17" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="AH17" s="29">
+      <c r="AG17" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH17" s="13">
         <v>-0.42</v>
       </c>
-      <c r="AI17" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ17" s="29">
+      <c r="AI17" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="AJ17" s="13">
         <v>-1.7</v>
       </c>
-      <c r="AK17" s="29">
+      <c r="AK17" s="13">
         <v>0.09</v>
       </c>
-      <c r="AL17" s="29">
+      <c r="AL17" s="13">
         <v>5</v>
       </c>
-      <c r="AM17" s="29">
+      <c r="AM17" s="13">
         <v>2</v>
       </c>
-      <c r="AN17" s="29">
+      <c r="AN17" s="13">
         <v>2</v>
       </c>
     </row>
@@ -10063,7 +10068,7 @@
         <v>77.55</v>
       </c>
       <c r="AI19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.2">
@@ -10074,7 +10079,7 @@
         <v>1.61</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>8</v>
@@ -10083,7 +10088,7 @@
         <v>0.01</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q20" s="5" t="s">
         <v>8</v>
@@ -10099,7 +10104,7 @@
         <v>0.35</v>
       </c>
       <c r="AA20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AG20" s="5" t="s">
         <v>8</v>
@@ -10108,7 +10113,7 @@
         <v>0.23</v>
       </c>
       <c r="AI20" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.2">
@@ -10588,13 +10593,13 @@
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="7">
         <v>0.03</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="D28" s="7">
         <v>0.28999999999999998</v>
@@ -10612,13 +10617,13 @@
         <v>32</v>
       </c>
       <c r="I28" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J28" s="26">
         <v>-0.04</v>
       </c>
       <c r="K28" s="27" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="L28" s="26">
         <v>-1.31</v>
@@ -10636,7 +10641,7 @@
         <v>19</v>
       </c>
       <c r="Q28" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R28" t="s">
         <v>26</v>
@@ -10660,13 +10665,13 @@
         <v>26</v>
       </c>
       <c r="Y28" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Z28" s="7">
         <v>0.05</v>
       </c>
       <c r="AA28" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AB28" s="7">
         <v>0.36</v>
@@ -10684,13 +10689,13 @@
         <v>47</v>
       </c>
       <c r="AG28" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH28" s="7">
         <v>0.06</v>
       </c>
       <c r="AI28" s="17" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="AJ28" s="7">
         <v>1.1499999999999999</v>
@@ -10710,13 +10715,13 @@
     </row>
     <row r="29" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B29" s="13">
         <v>-0.24</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="D29" s="13">
         <v>-1.27</v>
@@ -10734,13 +10739,13 @@
         <v>18</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="J29" s="13">
         <v>-0.01</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="L29" s="13">
         <v>-0.1</v>
@@ -10758,7 +10763,7 @@
         <v>3</v>
       </c>
       <c r="Q29" s="13" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="R29" s="15" t="s">
         <v>26</v>
@@ -10782,13 +10787,13 @@
         <v>26</v>
       </c>
       <c r="Y29" s="13" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="Z29" s="15">
         <v>0.06</v>
       </c>
       <c r="AA29" s="16" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="AB29" s="15">
         <v>0.59</v>
@@ -10806,13 +10811,13 @@
         <v>14</v>
       </c>
       <c r="AG29" s="13" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="AH29" s="15">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="AI29" s="16" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="AJ29" s="15">
         <v>-0.48</v>
@@ -10853,7 +10858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E0BD80-0BB3-E04A-A7FE-1D76F2CD0D51}">
   <dimension ref="A1:Y37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
@@ -10868,18 +10873,18 @@
   <sheetData>
     <row r="1" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
@@ -10996,10 +11001,10 @@
         <v>3.2</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="D8" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>8</v>
@@ -11008,10 +11013,10 @@
         <v>1.56</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="I8" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>8</v>
@@ -11023,7 +11028,7 @@
         <v>25</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>8</v>
@@ -11032,10 +11037,10 @@
         <v>1.36</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="U8" s="5" t="s">
         <v>8</v>
@@ -11047,7 +11052,7 @@
         <v>24</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
@@ -11438,13 +11443,13 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="B16">
         <v>-0.2</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="D16">
         <v>-1.1599999999999999</v>
@@ -11453,13 +11458,13 @@
         <v>0.25</v>
       </c>
       <c r="F16" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="G16">
         <v>-0.23</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="I16">
         <v>-0.81</v>
@@ -11468,13 +11473,13 @@
         <v>0.42</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="L16" s="4">
         <v>0.62</v>
       </c>
       <c r="M16" s="12" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="N16" s="4">
         <v>2.95</v>
@@ -11483,13 +11488,13 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="P16" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="Q16">
         <v>-0.05</v>
       </c>
       <c r="R16" s="10" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="S16">
         <v>-0.24</v>
@@ -11498,13 +11503,13 @@
         <v>0.81</v>
       </c>
       <c r="U16" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="V16">
         <v>0.66</v>
       </c>
       <c r="W16" s="10" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="X16">
         <v>1.2</v>
@@ -11515,13 +11520,13 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="B17">
         <v>-0.21</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="D17">
         <v>-1.19</v>
@@ -11530,13 +11535,13 @@
         <v>0.23</v>
       </c>
       <c r="F17" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="G17">
         <v>-0.11</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="I17">
         <v>-0.43</v>
@@ -11545,13 +11550,13 @@
         <v>0.67</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="L17" s="5">
         <v>0.66</v>
       </c>
       <c r="M17" s="11" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="N17" s="5">
         <v>1.76</v>
@@ -11560,13 +11565,13 @@
         <v>0.08</v>
       </c>
       <c r="P17" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="Q17" s="5">
         <v>0.23</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="S17" s="5">
         <v>1.1000000000000001</v>
@@ -11575,13 +11580,13 @@
         <v>0.27</v>
       </c>
       <c r="U17" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="V17">
         <v>0.8</v>
       </c>
       <c r="W17" s="10" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="X17">
         <v>1.21</v>
@@ -11592,13 +11597,13 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="B18">
         <v>-0.26</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="D18">
         <v>-1.1599999999999999</v>
@@ -11607,13 +11612,13 @@
         <v>0.11</v>
       </c>
       <c r="F18" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="G18">
         <v>-0.22</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="I18">
         <v>-0.82</v>
@@ -11622,13 +11627,13 @@
         <v>0.41</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="L18" s="4">
         <v>0.63</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="N18" s="4">
         <v>2.99</v>
@@ -11637,13 +11642,13 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="P18" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="Q18" s="5">
         <v>0.27</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="S18" s="5">
         <v>1.37</v>
@@ -11652,13 +11657,13 @@
         <v>0.17</v>
       </c>
       <c r="U18" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="V18">
         <v>0.78</v>
       </c>
       <c r="W18" s="10" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="X18">
         <v>1.6</v>
@@ -11669,13 +11674,13 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="B19" s="5">
         <v>0.03</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="D19" s="5">
         <v>0.18</v>
@@ -11684,13 +11689,13 @@
         <v>0.86</v>
       </c>
       <c r="F19" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="G19">
         <v>-0.11</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="I19">
         <v>-0.4</v>
@@ -11699,13 +11704,13 @@
         <v>0.69</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="L19" s="5">
         <v>0.33</v>
       </c>
       <c r="M19" s="11" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="N19" s="5">
         <v>1.3</v>
@@ -11714,13 +11719,13 @@
         <v>0.19</v>
       </c>
       <c r="P19" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="Q19" s="5">
         <v>0.17</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="S19" s="5">
         <v>0.82</v>
@@ -11729,13 +11734,13 @@
         <v>0.41</v>
       </c>
       <c r="U19" s="5" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="V19" s="5">
         <v>0.87</v>
       </c>
       <c r="W19" s="11" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="X19" s="5">
         <v>1.86</v>
@@ -11746,13 +11751,13 @@
     </row>
     <row r="20" spans="1:25" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="B20" s="22">
         <v>-0.74</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="D20" s="22">
         <v>-2.88</v>
@@ -11761,13 +11766,13 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="G20" s="20">
         <v>-0.47</v>
       </c>
       <c r="H20" s="21" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="I20" s="20">
         <v>-1.64</v>
@@ -11776,13 +11781,13 @@
         <v>0.1</v>
       </c>
       <c r="K20" s="20" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="L20" s="20">
         <v>0.75</v>
       </c>
       <c r="M20" s="21" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
       <c r="N20" s="20">
         <v>1.83</v>
@@ -11791,13 +11796,13 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="P20" s="24" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="Q20" s="20">
         <v>0.22</v>
       </c>
       <c r="R20" s="21" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="S20" s="20">
         <v>1.02</v>
@@ -11806,13 +11811,13 @@
         <v>0.31</v>
       </c>
       <c r="U20" s="24" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="V20" s="24">
         <v>0.6</v>
       </c>
       <c r="W20" s="25" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="X20" s="24">
         <v>1.1399999999999999</v>
@@ -11823,13 +11828,13 @@
     </row>
     <row r="21" spans="1:25" s="15" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B21" s="13">
         <v>0.01</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="D21" s="13">
         <v>0.69</v>
@@ -11838,13 +11843,13 @@
         <v>0.49</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="G21" s="15">
         <v>0.02</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="I21" s="15">
         <v>0.55000000000000004</v>
@@ -11853,13 +11858,13 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="K21" s="29" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="L21" s="29">
         <v>-0.08</v>
       </c>
       <c r="M21" s="30" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
       <c r="N21" s="29">
         <v>-2.84</v>
@@ -11868,13 +11873,13 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="P21" s="15" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="Q21" s="15">
         <v>-0.03</v>
       </c>
       <c r="R21" s="16" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="S21" s="15">
         <v>-1.04</v>
@@ -11883,13 +11888,13 @@
         <v>0.3</v>
       </c>
       <c r="U21" s="15" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="V21" s="15">
         <v>-0.23</v>
       </c>
       <c r="W21" s="16" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="X21" s="15">
         <v>-1.4</v>
@@ -11959,7 +11964,7 @@
         <v>73.63</v>
       </c>
       <c r="W23" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
@@ -11970,10 +11975,10 @@
         <v>0.99</v>
       </c>
       <c r="C24" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="D24" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>8</v>
@@ -11982,10 +11987,10 @@
         <v>0.98</v>
       </c>
       <c r="H24" t="s">
+        <v>96</v>
+      </c>
+      <c r="I24" t="s">
         <v>113</v>
-      </c>
-      <c r="I24" t="s">
-        <v>130</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>8</v>
@@ -11994,10 +11999,10 @@
         <v>0.87</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="P24" s="5" t="s">
         <v>8</v>
@@ -12006,10 +12011,10 @@
         <v>0.26</v>
       </c>
       <c r="R24" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="S24" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="U24" s="5" t="s">
         <v>8</v>
@@ -12018,10 +12023,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="W24" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="X24" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
@@ -12406,13 +12411,13 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="B32" s="7">
         <v>0.04</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="D32" s="7">
         <v>0.21</v>
@@ -12421,13 +12426,13 @@
         <v>0.83</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="G32" s="7">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="I32" s="7">
         <v>-0.67</v>
@@ -12436,13 +12441,13 @@
         <v>0.5</v>
       </c>
       <c r="K32" s="26" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="L32" s="26">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="M32" s="27" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="N32" s="26">
         <v>-0.84</v>
@@ -12451,13 +12456,13 @@
         <v>0.4</v>
       </c>
       <c r="P32" s="7" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="Q32" s="7">
         <v>0.08</v>
       </c>
       <c r="R32" s="17" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="S32" s="7">
         <v>0.48</v>
@@ -12466,13 +12471,13 @@
         <v>0.63</v>
       </c>
       <c r="U32" s="7" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="V32" s="7">
         <v>-0.14000000000000001</v>
       </c>
       <c r="W32" s="17" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="X32" s="7">
         <v>-0.43</v>
@@ -12483,13 +12488,13 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="24" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="B33" s="24">
         <v>-0.09</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="D33" s="24">
         <v>-0.48</v>
@@ -12498,13 +12503,13 @@
         <v>0.63</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="G33" s="20">
         <v>-0.15</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="I33" s="20">
         <v>-1.83</v>
@@ -12513,13 +12518,13 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K33" s="24" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="L33" s="24">
         <v>0.16</v>
       </c>
       <c r="M33" s="25" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="N33" s="24">
         <v>0.19</v>
@@ -12528,13 +12533,13 @@
         <v>0.85</v>
       </c>
       <c r="P33" s="24" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="Q33" s="24">
         <v>0.08</v>
       </c>
       <c r="R33" s="25" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="S33" s="24">
         <v>0.51</v>
@@ -12543,13 +12548,13 @@
         <v>0.61</v>
       </c>
       <c r="U33" s="20" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="V33" s="20">
         <v>0.32</v>
       </c>
       <c r="W33" s="21" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="X33" s="20">
         <v>1.24</v>
@@ -12560,13 +12565,13 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="24" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="B34" s="24">
         <v>-0.03</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="D34" s="24">
         <v>-0.18</v>
@@ -12575,13 +12580,13 @@
         <v>0.86</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="G34" s="24">
         <v>-0.06</v>
       </c>
       <c r="H34" s="25" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="I34" s="24">
         <v>-0.67</v>
@@ -12590,13 +12595,13 @@
         <v>0.5</v>
       </c>
       <c r="K34" s="24" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="L34" s="24">
         <v>-0.05</v>
       </c>
       <c r="M34" s="25" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="N34" s="24">
         <v>-0.3</v>
@@ -12605,13 +12610,13 @@
         <v>0.76</v>
       </c>
       <c r="P34" s="24" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="Q34" s="24">
         <v>0.03</v>
       </c>
       <c r="R34" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S34" s="24">
         <v>0.21</v>
@@ -12620,13 +12625,13 @@
         <v>0.83</v>
       </c>
       <c r="U34" s="24" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="V34" s="24">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="W34" s="25" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="X34" s="24">
         <v>0.28000000000000003</v>
@@ -12637,13 +12642,13 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="B35" s="20">
         <v>-0.27</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="D35" s="20">
         <v>-1.73</v>
@@ -12652,13 +12657,13 @@
         <v>0.08</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="G35" s="24">
         <v>-0.06</v>
       </c>
       <c r="H35" s="25" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="I35" s="24">
         <v>-0.68</v>
@@ -12667,13 +12672,13 @@
         <v>0.5</v>
       </c>
       <c r="K35" s="24" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="L35" s="24">
         <v>0.06</v>
       </c>
       <c r="M35" s="25" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="N35" s="24">
         <v>0.56000000000000005</v>
@@ -12682,13 +12687,13 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="P35" s="24" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="Q35" s="24">
         <v>0.01</v>
       </c>
       <c r="R35" s="25" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="S35" s="24">
         <v>0.09</v>
@@ -12697,13 +12702,13 @@
         <v>0.93</v>
       </c>
       <c r="U35" s="24" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="V35" s="24">
         <v>-0.13</v>
       </c>
       <c r="W35" s="25" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="X35" s="24">
         <v>-0.59</v>
@@ -12714,13 +12719,13 @@
     </row>
     <row r="36" spans="1:25" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="B36" s="24">
         <v>0.12</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="D36" s="24">
         <v>0.44</v>
@@ -12729,13 +12734,13 @@
         <v>0.66</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="G36" s="20">
         <v>0.03</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="I36" s="20">
         <v>0.28999999999999998</v>
@@ -12744,13 +12749,13 @@
         <v>0.77</v>
       </c>
       <c r="K36" s="20" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="L36" s="24">
         <v>0.26</v>
       </c>
       <c r="M36" s="25" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="N36" s="24">
         <v>1.41</v>
@@ -12759,13 +12764,13 @@
         <v>0.16</v>
       </c>
       <c r="P36" s="20" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="Q36" s="24">
         <v>0.03</v>
       </c>
       <c r="R36" s="25" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="S36" s="24">
         <v>0.2</v>
@@ -12774,13 +12779,13 @@
         <v>0.84</v>
       </c>
       <c r="U36" s="20" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="V36" s="24">
         <v>-0.14000000000000001</v>
       </c>
       <c r="W36" s="25" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="X36" s="24">
         <v>-0.4</v>
@@ -12791,13 +12796,13 @@
     </row>
     <row r="37" spans="1:25" s="15" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="38" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B37" s="15">
         <v>0</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="D37" s="15">
         <v>0.26</v>
@@ -12806,13 +12811,13 @@
         <v>0.8</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="G37" s="15">
         <v>0.01</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="I37" s="15">
         <v>0.46</v>
@@ -12821,13 +12826,13 @@
         <v>0.65</v>
       </c>
       <c r="K37" s="15" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="L37" s="15">
         <v>0</v>
       </c>
       <c r="M37" s="16" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="N37" s="15">
         <v>-0.03</v>
@@ -12836,13 +12841,13 @@
         <v>0.97</v>
       </c>
       <c r="P37" s="15" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="Q37" s="15">
         <v>0.01</v>
       </c>
       <c r="R37" s="16" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="S37" s="15">
         <v>0.51</v>
@@ -12851,13 +12856,13 @@
         <v>0.61</v>
       </c>
       <c r="U37" s="15" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="V37" s="15">
         <v>0.01</v>
       </c>
       <c r="W37" s="16" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="X37" s="15">
         <v>0.12</v>
@@ -12883,23 +12888,23 @@
   <sheetData>
     <row r="1" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:40" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -13026,7 +13031,7 @@
         <v>0.25</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>8</v>
@@ -13035,7 +13040,7 @@
         <v>0.62</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="Q8" s="4" t="s">
         <v>8</v>
@@ -13044,10 +13049,10 @@
         <v>4.45</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="T8" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>8</v>
@@ -13056,7 +13061,7 @@
         <v>2.64</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="AG8" s="5" t="s">
         <v>8</v>
@@ -13065,7 +13070,7 @@
         <v>0.17</v>
       </c>
       <c r="AI8" s="5" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
@@ -13546,13 +13551,13 @@
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16">
         <v>-0.12</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="D16">
         <v>-1.02</v>
@@ -13570,13 +13575,13 @@
         <v>40</v>
       </c>
       <c r="I16" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J16" s="28">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L16" s="28">
         <v>-0.4</v>
@@ -13594,13 +13599,13 @@
         <v>36</v>
       </c>
       <c r="Q16" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R16" s="4">
         <v>0.3</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="T16" s="4">
         <v>2.12</v>
@@ -13618,13 +13623,13 @@
         <v>37</v>
       </c>
       <c r="Y16" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Z16" s="5">
         <v>0.13</v>
       </c>
       <c r="AA16" s="11" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="AB16" s="5">
         <v>0.75</v>
@@ -13642,13 +13647,13 @@
         <v>48</v>
       </c>
       <c r="AG16" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH16" s="28">
         <v>0.06</v>
       </c>
       <c r="AI16" s="10" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
       <c r="AJ16" s="28">
         <v>0.7</v>
@@ -13668,13 +13673,13 @@
     </row>
     <row r="17" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="B17" s="13">
         <v>-0.06</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="D17" s="13">
         <v>-0.5</v>
@@ -13692,13 +13697,13 @@
         <v>16</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="J17" s="13">
         <v>0.08</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="L17" s="13">
         <v>0.79</v>
@@ -13716,13 +13721,13 @@
         <v>10</v>
       </c>
       <c r="Q17" s="29" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="R17" s="29">
         <v>-0.28999999999999998</v>
       </c>
       <c r="S17" s="30" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="T17" s="29">
         <v>-2.11</v>
@@ -13740,13 +13745,13 @@
         <v>11</v>
       </c>
       <c r="Y17" s="13" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="Z17" s="13">
         <v>-0.21</v>
       </c>
       <c r="AA17" s="14" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="AB17" s="13">
         <v>-1.62</v>
@@ -13764,13 +13769,13 @@
         <v>16</v>
       </c>
       <c r="AG17" s="13" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="AH17" s="13">
         <v>-0.42</v>
       </c>
       <c r="AI17" s="14" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="AJ17" s="13">
         <v>0.42</v>
@@ -13849,7 +13854,7 @@
         <v>77.56</v>
       </c>
       <c r="AI19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.2">
@@ -13860,7 +13865,7 @@
         <v>0.02</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>8</v>
@@ -13869,7 +13874,7 @@
         <v>1.32</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="Q20" s="5" t="s">
         <v>8</v>
@@ -13878,7 +13883,7 @@
         <v>1.92</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
       <c r="Y20" s="5" t="s">
         <v>8</v>
@@ -13887,7 +13892,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="AA20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG20" s="5" t="s">
         <v>8</v>
@@ -13896,7 +13901,7 @@
         <v>0.23</v>
       </c>
       <c r="AI20" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.2">
@@ -14376,13 +14381,13 @@
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="7">
         <v>-0.15</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="D28" s="7">
         <v>-0.56999999999999995</v>
@@ -14400,13 +14405,13 @@
         <v>40</v>
       </c>
       <c r="I28" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J28" s="26">
         <v>-0.03</v>
       </c>
       <c r="K28" s="27" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="L28" s="26">
         <v>-0.98</v>
@@ -14424,13 +14429,13 @@
         <v>36</v>
       </c>
       <c r="Q28" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R28">
         <v>0</v>
       </c>
       <c r="S28" s="10" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="T28">
         <v>0</v>
@@ -14448,13 +14453,13 @@
         <v>37</v>
       </c>
       <c r="Y28" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Z28" s="7">
         <v>0.08</v>
       </c>
       <c r="AA28" s="17" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="AB28" s="7">
         <v>0.55000000000000004</v>
@@ -14472,13 +14477,13 @@
         <v>48</v>
       </c>
       <c r="AG28" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH28" s="7">
         <v>0.06</v>
       </c>
       <c r="AI28" s="17" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="AJ28" s="7">
         <v>1.1499999999999999</v>
@@ -14498,13 +14503,13 @@
     </row>
     <row r="29" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="B29" s="13">
         <v>0.02</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
       <c r="D29" s="13">
         <v>0.16</v>
@@ -14522,13 +14527,13 @@
         <v>16</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="J29" s="13">
         <v>-0.08</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
       <c r="L29" s="13">
         <v>-1.1499999999999999</v>
@@ -14546,13 +14551,13 @@
         <v>10</v>
       </c>
       <c r="Q29" s="13" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="R29" s="15">
         <v>-0.11</v>
       </c>
       <c r="S29" s="16" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="T29" s="15">
         <v>-1.38</v>
@@ -14570,13 +14575,13 @@
         <v>11</v>
       </c>
       <c r="Y29" s="13" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="Z29" s="15">
         <v>-0.03</v>
       </c>
       <c r="AA29" s="16" t="s">
-        <v>289</v>
+        <v>271</v>
       </c>
       <c r="AB29" s="15">
         <v>-0.38</v>
@@ -14594,13 +14599,13 @@
         <v>16</v>
       </c>
       <c r="AG29" s="13" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="AH29" s="15">
         <v>-0.09</v>
       </c>
       <c r="AI29" s="16" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="AJ29" s="15">
         <v>-0.48</v>

</xml_diff>